<commit_message>
Soil Surface Texture Class by Thickness (not depth)
Soil Surface Texture Class by Thickness (not depth):
</commit_message>
<xml_diff>
--- a/documents/Soil grouping_gSSURGO_forCEAP-GL_FINAL_11-25-2019.xlsx
+++ b/documents/Soil grouping_gSSURGO_forCEAP-GL_FINAL_11-25-2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\CEAP-Grazing-Lands\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A026539D-7FA5-4E62-B532-9B20C9E6BF44}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D14075-FDDF-47CC-97DC-E98F3B6DA3F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CEAP-GL SSURGO soil for APEX" sheetId="1" r:id="rId1"/>
@@ -3108,21 +3108,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">IF ((om_r &gt;= 18*1.724 and claytotal_r &gt;= 60) or ((om_r &gt;=(12 +(claytotal_r*0.1))*1.724) and claytotal_r &lt; 60) or  om_r &gt;= 20*1.724) and not isnull(claytotal_r) and not isnull(om_r) THEN "yes" .                                                                               </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>THIS CALCULATION WILL OVERRIDE ANY VALUE FOUND IN DESGNMASTER.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Need to split into top depths of when the diagnostic horizon kind is encountered:  "Depth1" is when the diag horiz kind is rather shallow.  "Depth2" is when the diag horiz kind is not shallow. Cokey is the link to this table.</t>
     </r>
     <r>
@@ -3141,6 +3126,21 @@
   </si>
   <si>
     <t xml:space="preserve">Queried for Wet soils. Moist/Dry would be interered differently based on east vs west but could be populated based on moisture. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">IF ((om_r &gt;= 18*1.724 and claytotal_r &gt;= 60) or ((om_r &gt;=(12 +(claytotal_r*0.1))*1.724) and claytotal_r &lt; 60) or  om_r &gt;= 20*1.724) and not isnull(claytotal_r) and not isnull(om_r) THEN "yes" .  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>THIS CALCULATION WILL OVERRIDE ANY VALUE FOUND IN DESGNMASTER.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3779,6 +3779,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3813,15 +3822,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4142,8 +4142,8 @@
   <dimension ref="A1:J81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -4174,21 +4174,21 @@
       <c r="D1" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="76" t="s">
+      <c r="E1" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="78"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="81"/>
       <c r="I1" s="39" t="s">
         <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="112.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="70" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="40" t="s">
@@ -4228,7 +4228,7 @@
       <c r="I3" s="44"/>
     </row>
     <row r="4" spans="1:10" ht="168.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="72" t="s">
         <v>126</v>
       </c>
       <c r="B4" s="40" t="s">
@@ -4243,10 +4243,10 @@
       <c r="E4" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="F4" s="83" t="s">
+      <c r="F4" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="G4" s="83" t="s">
+      <c r="G4" s="71" t="s">
         <v>125</v>
       </c>
       <c r="H4" s="40"/>
@@ -4254,7 +4254,7 @@
         <v>233</v>
       </c>
       <c r="J4" s="45" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -4278,7 +4278,7 @@
       <c r="J5" s="45"/>
     </row>
     <row r="6" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="84" t="s">
+      <c r="A6" s="72" t="s">
         <v>260</v>
       </c>
       <c r="B6" s="40" t="s">
@@ -4319,7 +4319,7 @@
       <c r="I7" s="44"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="84" t="s">
+      <c r="A8" s="72" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="40" t="s">
@@ -4338,7 +4338,7 @@
       <c r="I8" s="53"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="84" t="s">
+      <c r="A9" s="72" t="s">
         <v>60</v>
       </c>
       <c r="B9" s="40" t="s">
@@ -4389,7 +4389,7 @@
       <c r="I11" s="53"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="84" t="s">
+      <c r="A12" s="72" t="s">
         <v>57</v>
       </c>
       <c r="B12" s="40" t="s">
@@ -4408,7 +4408,7 @@
       <c r="I12" s="53"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="84" t="s">
+      <c r="A13" s="72" t="s">
         <v>58</v>
       </c>
       <c r="B13" s="40" t="s">
@@ -4427,7 +4427,7 @@
       <c r="I13" s="53"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="84" t="s">
+      <c r="A14" s="72" t="s">
         <v>59</v>
       </c>
       <c r="B14" s="40" t="s">
@@ -4474,7 +4474,7 @@
       <c r="I16" s="44"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="84" t="s">
+      <c r="A17" s="72" t="s">
         <v>55</v>
       </c>
       <c r="B17" s="40" t="s">
@@ -4492,13 +4492,13 @@
       <c r="F17" s="40"/>
       <c r="G17" s="40"/>
       <c r="H17" s="40"/>
-      <c r="I17" s="73" t="s">
+      <c r="I17" s="76" t="s">
         <v>26</v>
       </c>
       <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="84" t="s">
+      <c r="A18" s="72" t="s">
         <v>54</v>
       </c>
       <c r="B18" s="40" t="s">
@@ -4516,11 +4516,11 @@
       <c r="F18" s="40"/>
       <c r="G18" s="40"/>
       <c r="H18" s="40"/>
-      <c r="I18" s="81"/>
+      <c r="I18" s="84"/>
       <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="84" t="s">
+      <c r="A19" s="72" t="s">
         <v>53</v>
       </c>
       <c r="B19" s="40" t="s">
@@ -4538,11 +4538,11 @@
       <c r="F19" s="40"/>
       <c r="G19" s="40"/>
       <c r="H19" s="40"/>
-      <c r="I19" s="81"/>
+      <c r="I19" s="84"/>
       <c r="J19" s="47"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="84" t="s">
+      <c r="A20" s="72" t="s">
         <v>52</v>
       </c>
       <c r="B20" s="40" t="s">
@@ -4560,7 +4560,7 @@
       <c r="F20" s="40"/>
       <c r="G20" s="40"/>
       <c r="H20" s="40"/>
-      <c r="I20" s="74"/>
+      <c r="I20" s="77"/>
       <c r="J20" s="47"/>
     </row>
     <row r="21" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -4583,7 +4583,7 @@
       <c r="I21" s="44"/>
     </row>
     <row r="22" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="84" t="s">
+      <c r="A22" s="72" t="s">
         <v>51</v>
       </c>
       <c r="B22" s="40" t="s">
@@ -4605,11 +4605,11 @@
         <v>132</v>
       </c>
       <c r="H22" s="40"/>
-      <c r="I22" s="73"/>
+      <c r="I22" s="76"/>
       <c r="J22" s="47"/>
     </row>
     <row r="23" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="84" t="s">
+      <c r="A23" s="72" t="s">
         <v>50</v>
       </c>
       <c r="B23" s="40" t="s">
@@ -4631,7 +4631,7 @@
         <v>132</v>
       </c>
       <c r="H23" s="40"/>
-      <c r="I23" s="74"/>
+      <c r="I23" s="77"/>
       <c r="J23" s="47"/>
     </row>
     <row r="24" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -4654,7 +4654,7 @@
       <c r="I24" s="44"/>
     </row>
     <row r="25" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="84" t="s">
+      <c r="A25" s="72" t="s">
         <v>49</v>
       </c>
       <c r="B25" s="40" t="s">
@@ -4680,7 +4680,7 @@
       <c r="J25" s="47"/>
     </row>
     <row r="26" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="84" t="s">
+      <c r="A26" s="72" t="s">
         <v>968</v>
       </c>
       <c r="B26" s="40" t="s">
@@ -4719,7 +4719,7 @@
       <c r="I27" s="44"/>
     </row>
     <row r="28" spans="1:10" ht="117.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="84" t="s">
+      <c r="A28" s="72" t="s">
         <v>113</v>
       </c>
       <c r="B28" s="40" t="s">
@@ -4735,13 +4735,13 @@
       <c r="F28" s="40"/>
       <c r="G28" s="40"/>
       <c r="H28" s="40"/>
-      <c r="I28" s="73" t="s">
-        <v>969</v>
-      </c>
-      <c r="J28" s="75"/>
+      <c r="I28" s="76" t="s">
+        <v>972</v>
+      </c>
+      <c r="J28" s="78"/>
     </row>
     <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="84" t="s">
+      <c r="A29" s="72" t="s">
         <v>120</v>
       </c>
       <c r="B29" s="40" t="s">
@@ -4757,11 +4757,11 @@
       <c r="F29" s="40"/>
       <c r="G29" s="40"/>
       <c r="H29" s="40"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="75"/>
+      <c r="I29" s="77"/>
+      <c r="J29" s="78"/>
     </row>
     <row r="30" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="84" t="s">
+      <c r="A30" s="72" t="s">
         <v>121</v>
       </c>
       <c r="B30" s="40" t="s">
@@ -4780,7 +4780,7 @@
       <c r="I30" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="J30" s="75"/>
+      <c r="J30" s="78"/>
     </row>
     <row r="31" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A31" s="58" t="s">
@@ -4821,7 +4821,7 @@
       <c r="F32" s="46"/>
       <c r="G32" s="46"/>
       <c r="H32" s="46"/>
-      <c r="I32" s="73" t="s">
+      <c r="I32" s="76" t="s">
         <v>263</v>
       </c>
       <c r="J32" s="52"/>
@@ -4845,7 +4845,7 @@
       <c r="F33" s="46"/>
       <c r="G33" s="46"/>
       <c r="H33" s="46"/>
-      <c r="I33" s="81"/>
+      <c r="I33" s="84"/>
       <c r="J33" s="52"/>
     </row>
     <row r="34" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -4867,7 +4867,7 @@
       </c>
       <c r="G34" s="46"/>
       <c r="H34" s="46"/>
-      <c r="I34" s="81"/>
+      <c r="I34" s="84"/>
       <c r="J34" s="52"/>
     </row>
     <row r="35" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -4889,7 +4889,7 @@
         <v>82</v>
       </c>
       <c r="H35" s="46"/>
-      <c r="I35" s="81"/>
+      <c r="I35" s="84"/>
       <c r="J35" s="52"/>
     </row>
     <row r="36" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -4911,7 +4911,7 @@
       <c r="H36" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="I36" s="81"/>
+      <c r="I36" s="84"/>
       <c r="J36" s="52"/>
     </row>
     <row r="37" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -4931,7 +4931,7 @@
       <c r="F37" s="46"/>
       <c r="G37" s="46"/>
       <c r="H37" s="46"/>
-      <c r="I37" s="81"/>
+      <c r="I37" s="84"/>
       <c r="J37" s="52"/>
     </row>
     <row r="38" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -4953,7 +4953,7 @@
       <c r="F38" s="46"/>
       <c r="G38" s="46"/>
       <c r="H38" s="46"/>
-      <c r="I38" s="81"/>
+      <c r="I38" s="84"/>
       <c r="J38" s="52"/>
     </row>
     <row r="39" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -4975,7 +4975,7 @@
       </c>
       <c r="G39" s="46"/>
       <c r="H39" s="46"/>
-      <c r="I39" s="81"/>
+      <c r="I39" s="84"/>
       <c r="J39" s="52"/>
     </row>
     <row r="40" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -4997,7 +4997,7 @@
         <v>82</v>
       </c>
       <c r="H40" s="46"/>
-      <c r="I40" s="81"/>
+      <c r="I40" s="84"/>
       <c r="J40" s="52"/>
     </row>
     <row r="41" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -5019,7 +5019,7 @@
       <c r="H41" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="I41" s="81"/>
+      <c r="I41" s="84"/>
       <c r="J41" s="52"/>
     </row>
     <row r="42" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -5041,7 +5041,7 @@
       <c r="F42" s="46"/>
       <c r="G42" s="46"/>
       <c r="H42" s="46"/>
-      <c r="I42" s="81"/>
+      <c r="I42" s="84"/>
       <c r="J42" s="52"/>
     </row>
     <row r="43" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -5063,7 +5063,7 @@
       <c r="F43" s="46"/>
       <c r="G43" s="46"/>
       <c r="H43" s="46"/>
-      <c r="I43" s="81"/>
+      <c r="I43" s="84"/>
       <c r="J43" s="52"/>
     </row>
     <row r="44" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -5085,7 +5085,7 @@
       <c r="F44" s="46"/>
       <c r="G44" s="46"/>
       <c r="H44" s="46"/>
-      <c r="I44" s="74"/>
+      <c r="I44" s="77"/>
       <c r="J44" s="52"/>
     </row>
     <row r="45" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -5126,8 +5126,8 @@
       </c>
       <c r="G46" s="40"/>
       <c r="H46" s="40"/>
-      <c r="I46" s="70" t="s">
-        <v>970</v>
+      <c r="I46" s="73" t="s">
+        <v>969</v>
       </c>
       <c r="J46" s="47"/>
     </row>
@@ -5152,7 +5152,7 @@
       </c>
       <c r="G47" s="40"/>
       <c r="H47" s="40"/>
-      <c r="I47" s="71"/>
+      <c r="I47" s="74"/>
     </row>
     <row r="48" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A48" s="62" t="s">
@@ -5175,7 +5175,7 @@
       </c>
       <c r="G48" s="40"/>
       <c r="H48" s="40"/>
-      <c r="I48" s="71"/>
+      <c r="I48" s="74"/>
     </row>
     <row r="49" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A49" s="62" t="s">
@@ -5198,7 +5198,7 @@
       </c>
       <c r="G49" s="40"/>
       <c r="H49" s="40"/>
-      <c r="I49" s="71"/>
+      <c r="I49" s="74"/>
     </row>
     <row r="50" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A50" s="62" t="s">
@@ -5221,7 +5221,7 @@
       </c>
       <c r="G50" s="40"/>
       <c r="H50" s="40"/>
-      <c r="I50" s="71"/>
+      <c r="I50" s="74"/>
     </row>
     <row r="51" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A51" s="62" t="s">
@@ -5244,7 +5244,7 @@
       </c>
       <c r="G51" s="40"/>
       <c r="H51" s="40"/>
-      <c r="I51" s="71"/>
+      <c r="I51" s="74"/>
     </row>
     <row r="52" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A52" s="62" t="s">
@@ -5267,7 +5267,7 @@
       </c>
       <c r="G52" s="40"/>
       <c r="H52" s="40"/>
-      <c r="I52" s="71"/>
+      <c r="I52" s="74"/>
     </row>
     <row r="53" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A53" s="62" t="s">
@@ -5290,7 +5290,7 @@
       </c>
       <c r="G53" s="40"/>
       <c r="H53" s="40"/>
-      <c r="I53" s="71"/>
+      <c r="I53" s="74"/>
     </row>
     <row r="54" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A54" s="62" t="s">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="G54" s="40"/>
       <c r="H54" s="40"/>
-      <c r="I54" s="71"/>
+      <c r="I54" s="74"/>
     </row>
     <row r="55" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A55" s="62" t="s">
@@ -5336,7 +5336,7 @@
       </c>
       <c r="G55" s="40"/>
       <c r="H55" s="40"/>
-      <c r="I55" s="80"/>
+      <c r="I55" s="83"/>
     </row>
     <row r="56" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A56" s="66" t="s">
@@ -5395,10 +5395,10 @@
       <c r="F58" s="40"/>
       <c r="G58" s="40"/>
       <c r="H58" s="40"/>
-      <c r="I58" s="70" t="s">
+      <c r="I58" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="J58" s="79"/>
+      <c r="J58" s="82"/>
     </row>
     <row r="59" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A59" s="62" t="s">
@@ -5419,8 +5419,8 @@
       <c r="F59" s="40"/>
       <c r="G59" s="40"/>
       <c r="H59" s="40"/>
-      <c r="I59" s="71"/>
-      <c r="J59" s="79"/>
+      <c r="I59" s="74"/>
+      <c r="J59" s="82"/>
     </row>
     <row r="60" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A60" s="62" t="s">
@@ -5441,8 +5441,8 @@
       <c r="F60" s="40"/>
       <c r="G60" s="40"/>
       <c r="H60" s="40"/>
-      <c r="I60" s="71"/>
-      <c r="J60" s="79"/>
+      <c r="I60" s="74"/>
+      <c r="J60" s="82"/>
     </row>
     <row r="61" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="62" t="s">
@@ -5463,8 +5463,8 @@
       <c r="F61" s="40"/>
       <c r="G61" s="40"/>
       <c r="H61" s="40"/>
-      <c r="I61" s="71"/>
-      <c r="J61" s="79"/>
+      <c r="I61" s="74"/>
+      <c r="J61" s="82"/>
     </row>
     <row r="62" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A62" s="62" t="s">
@@ -5485,8 +5485,8 @@
       <c r="F62" s="40"/>
       <c r="G62" s="40"/>
       <c r="H62" s="40"/>
-      <c r="I62" s="80"/>
-      <c r="J62" s="79"/>
+      <c r="I62" s="83"/>
+      <c r="J62" s="82"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="58" t="s">
@@ -5520,7 +5520,7 @@
       <c r="G64" s="40"/>
       <c r="H64" s="40"/>
       <c r="I64" s="53"/>
-      <c r="J64" s="79"/>
+      <c r="J64" s="82"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="62" t="s">
@@ -5540,7 +5540,7 @@
       <c r="G65" s="40"/>
       <c r="H65" s="40"/>
       <c r="I65" s="53"/>
-      <c r="J65" s="79"/>
+      <c r="J65" s="82"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="62" t="s">
@@ -5560,7 +5560,7 @@
       <c r="G66" s="40"/>
       <c r="H66" s="40"/>
       <c r="I66" s="53"/>
-      <c r="J66" s="79"/>
+      <c r="J66" s="82"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="62" t="s">
@@ -5580,7 +5580,7 @@
       <c r="G67" s="40"/>
       <c r="H67" s="40"/>
       <c r="I67" s="53"/>
-      <c r="J67" s="79"/>
+      <c r="J67" s="82"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="62" t="s">
@@ -5600,7 +5600,7 @@
       <c r="G68" s="40"/>
       <c r="H68" s="40"/>
       <c r="I68" s="53"/>
-      <c r="J68" s="79"/>
+      <c r="J68" s="82"/>
     </row>
     <row r="69" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A69" s="58" t="s">
@@ -5648,7 +5648,7 @@
       <c r="H70" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="I70" s="70" t="s">
+      <c r="I70" s="73" t="s">
         <v>269</v>
       </c>
     </row>
@@ -5677,7 +5677,7 @@
       <c r="H71" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="I71" s="71"/>
+      <c r="I71" s="74"/>
     </row>
     <row r="72" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A72" s="62" t="s">
@@ -5704,7 +5704,7 @@
       <c r="H72" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="I72" s="71"/>
+      <c r="I72" s="74"/>
     </row>
     <row r="73" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A73" s="62" t="s">
@@ -5731,7 +5731,7 @@
       <c r="H73" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="I73" s="71"/>
+      <c r="I73" s="74"/>
     </row>
     <row r="74" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A74" s="62" t="s">
@@ -5758,7 +5758,7 @@
       <c r="H74" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="I74" s="71"/>
+      <c r="I74" s="74"/>
     </row>
     <row r="75" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A75" s="62" t="s">
@@ -5785,7 +5785,7 @@
       <c r="H75" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="I75" s="71"/>
+      <c r="I75" s="74"/>
     </row>
     <row r="76" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A76" s="62" t="s">
@@ -5812,7 +5812,7 @@
       <c r="H76" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="I76" s="71"/>
+      <c r="I76" s="74"/>
     </row>
     <row r="77" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A77" s="62" t="s">
@@ -5839,7 +5839,7 @@
       <c r="H77" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="I77" s="71"/>
+      <c r="I77" s="74"/>
     </row>
     <row r="78" spans="1:10" ht="57" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="68" t="s">
@@ -5866,7 +5866,7 @@
       <c r="H78" s="69" t="s">
         <v>131</v>
       </c>
-      <c r="I78" s="72"/>
+      <c r="I78" s="75"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E79" s="45"/>
@@ -6337,7 +6337,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="24.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="35" t="s">
         <v>344</v>
       </c>
@@ -6354,7 +6354,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="24.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="35" t="s">
         <v>347</v>
       </c>
@@ -6558,7 +6558,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="24.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="35" t="s">
         <v>371</v>
       </c>
@@ -10998,8 +10998,8 @@
   </sheetPr>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>